<commit_message>
Updated Insights to data
</commit_message>
<xml_diff>
--- a/Results&Visualisations/Visualisation.xlsx
+++ b/Results&Visualisations/Visualisation.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f9f4b9a8d9f2c4fd/Desktop/Developer/SQL_Job_Analysis/SQL_Job_Analysis_Project/Results^0Visualisations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FF59BDBE-C1CB-4180-B60D-234B42BE20E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="8_{FF59BDBE-C1CB-4180-B60D-234B42BE20E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A704304-B2FA-456D-B9D3-28C3FCCD4486}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{C90E4D22-8C84-4BE8-9F10-F300437C0791}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="4" xr2:uid="{C90E4D22-8C84-4BE8-9F10-F300437C0791}"/>
   </bookViews>
   <sheets>
     <sheet name="1. Singapore" sheetId="1" r:id="rId1"/>
     <sheet name="1. Remote" sheetId="2" r:id="rId2"/>
+    <sheet name="2" sheetId="3" r:id="rId3"/>
+    <sheet name="4. Top_paying_skills" sheetId="4" r:id="rId4"/>
+    <sheet name="5. Optimal_skills" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="70">
   <si>
     <t>Fraud Data Analyst</t>
   </si>
@@ -172,6 +175,81 @@
   </si>
   <si>
     <t>Get It Recruit - Information Technology</t>
+  </si>
+  <si>
+    <t>skills</t>
+  </si>
+  <si>
+    <t>skill_count</t>
+  </si>
+  <si>
+    <t>sql</t>
+  </si>
+  <si>
+    <t>excel</t>
+  </si>
+  <si>
+    <t>python</t>
+  </si>
+  <si>
+    <t>tableau</t>
+  </si>
+  <si>
+    <t>power bi</t>
+  </si>
+  <si>
+    <t>avg_salary</t>
+  </si>
+  <si>
+    <t>svn</t>
+  </si>
+  <si>
+    <t>solidity</t>
+  </si>
+  <si>
+    <t>couchbase</t>
+  </si>
+  <si>
+    <t>datarobot</t>
+  </si>
+  <si>
+    <t>golang</t>
+  </si>
+  <si>
+    <t>mxnet</t>
+  </si>
+  <si>
+    <t>dplyr</t>
+  </si>
+  <si>
+    <t>vmware</t>
+  </si>
+  <si>
+    <t>terraform</t>
+  </si>
+  <si>
+    <t>twilio</t>
+  </si>
+  <si>
+    <t>skill_id</t>
+  </si>
+  <si>
+    <t>kafka</t>
+  </si>
+  <si>
+    <t>pytorch</t>
+  </si>
+  <si>
+    <t>perl</t>
+  </si>
+  <si>
+    <t>tensorflow</t>
+  </si>
+  <si>
+    <t>cassandra</t>
+  </si>
+  <si>
+    <t>atlassian</t>
   </si>
 </sst>
 </file>
@@ -210,15 +288,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
@@ -945,6 +1027,1410 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Top 5 Highest demanded Data Analyst</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> skills</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2'!$A$2:$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>sql</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>excel</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>python</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>tableau</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>power bi</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2'!$B$2:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>92628</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>67031</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>57326</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>46554</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>39468</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-26E8-4C2C-819C-61D3EEBEE6BA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="929253567"/>
+        <c:axId val="929250687"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="929253567"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="929250687"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="929250687"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="929253567"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Top-10-Paying</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Skills</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'4. Top_paying_skills'!$A$2:$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>svn</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>solidity</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>couchbase</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>datarobot</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>golang</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>mxnet</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>dplyr</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>vmware</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>terraform</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>twilio</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'4. Top_paying_skills'!$B$2:$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>400000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>179000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>160515</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>155486</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>155000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>149000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>147633</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>147500</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>146734</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>138500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D6A1-449D-9703-564C10F685A5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="984314303"/>
+        <c:axId val="984323423"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="984314303"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="984323423"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="984323423"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="984314303"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Skill Count</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs Average Salary</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{29C53E27-DE67-4F01-8CBC-5B1DA6E68863}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-F833-44AA-BEDB-9CFC2E0E70E0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{4096B0B6-E531-443C-BD0B-CC06AA541287}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-F833-44AA-BEDB-9CFC2E0E70E0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{A6389461-959C-4C42-BA01-29E4B22D48E4}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-F833-44AA-BEDB-9CFC2E0E70E0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{2692C954-3DAE-4C20-8881-4C8EA1D819C5}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-F833-44AA-BEDB-9CFC2E0E70E0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{2B5CEB56-12FA-4A8B-B4C4-1D79DCB3C00C}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-F833-44AA-BEDB-9CFC2E0E70E0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{726BCF31-E5A7-4C3D-8F5E-3E897D176848}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[CELLRANGE]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000006-F833-44AA-BEDB-9CFC2E0E70E0}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showDataLabelsRange val="1"/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'5. Optimal_skills'!$C$2:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'5. Optimal_skills'!$D$2:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>129999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>125226</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>124686</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>120647</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>118407</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>117966</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:datalabelsRange>
+                <c15:f>'5. Optimal_skills'!$B$2:$B$7</c15:f>
+                <c15:dlblRangeCache>
+                  <c:ptCount val="6"/>
+                  <c:pt idx="0">
+                    <c:v>kafka</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>pytorch</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>perl</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>tensorflow</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>cassandra</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>atlassian</c:v>
+                  </c:pt>
+                </c15:dlblRangeCache>
+              </c15:datalabelsRange>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F833-44AA-BEDB-9CFC2E0E70E0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="984320063"/>
+        <c:axId val="984307103"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="984320063"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Skill Count</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="984307103"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="984307103"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Average Salary</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="984320063"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1025,6 +2511,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
@@ -2016,6 +3622,1532 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -2117,15 +5249,138 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F1684F8-83B2-9FEA-1442-27DFB7AEFEC1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>4762</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>309562</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A376C4CB-1CAE-9EEB-5E26-D3FDC6900762}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>528637</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>52386</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F8A3E66-34F1-5EBD-F44A-EC14B7AA8E5A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EE8CC734-FE31-49F1-94A2-B15AC21A8298}" name="Table1" displayName="Table1" ref="A1:E11" totalsRowShown="0">
   <autoFilter ref="A1:E11" xr:uid="{EE8CC734-FE31-49F1-94A2-B15AC21A8298}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{8E9B90D9-C976-4FE0-950F-B7467839B69C}" name="job_title" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{34A5D547-15D8-48E9-94C1-623F7A544623}" name="company_name" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{06F6328C-4920-40A3-A768-9807460CD4D4}" name="job_location" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{D105852C-E2EA-4CD9-8310-3A77D415FB08}" name="job_schedule_type" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{99030DDF-A156-472A-B268-30646CFB7846}" name="salary_year_avg" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{8E9B90D9-C976-4FE0-950F-B7467839B69C}" name="job_title" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{34A5D547-15D8-48E9-94C1-623F7A544623}" name="company_name" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{06F6328C-4920-40A3-A768-9807460CD4D4}" name="job_location" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{D105852C-E2EA-4CD9-8310-3A77D415FB08}" name="job_schedule_type" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{99030DDF-A156-472A-B268-30646CFB7846}" name="salary_year_avg" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2140,6 +5395,41 @@
     <tableColumn id="3" xr3:uid="{2C4CE807-AFA2-430F-A143-9C0CD269DF8A}" name="remote_job"/>
     <tableColumn id="4" xr3:uid="{EA311A11-9621-4D34-A3E5-4C44CB9EAE26}" name="job_schedule_type"/>
     <tableColumn id="5" xr3:uid="{BB949899-0520-4628-859F-6D7DF0B34870}" name="salary_year_avg"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3C811004-1203-42DE-B482-E7B41B9FE813}" name="Table3" displayName="Table3" ref="A1:B6" totalsRowShown="0">
+  <autoFilter ref="A1:B6" xr:uid="{3C811004-1203-42DE-B482-E7B41B9FE813}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{74875538-F82D-4F6C-88B9-DEF9D9DEAC9B}" name="skills"/>
+    <tableColumn id="2" xr3:uid="{62F2DA38-D124-4486-9266-0E4A0E7E43E8}" name="skill_count" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A9B03FFA-955C-4595-8CD7-9C7054F4DA84}" name="Table4" displayName="Table4" ref="A1:B11" totalsRowShown="0">
+  <autoFilter ref="A1:B11" xr:uid="{A9B03FFA-955C-4595-8CD7-9C7054F4DA84}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{380E7ED1-69ED-4BAE-8357-EE9289C9998F}" name="skills"/>
+    <tableColumn id="2" xr3:uid="{341A66BD-3C6D-4A77-84D0-D0904C4CAAC5}" name="avg_salary"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E9A7685C-B801-47BD-AC0B-8A1A94F0637A}" name="Table5" displayName="Table5" ref="A1:D7" totalsRowShown="0">
+  <autoFilter ref="A1:D7" xr:uid="{E9A7685C-B801-47BD-AC0B-8A1A94F0637A}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{763A9376-4ED5-4661-9CFA-53EC945E4C7A}" name="skill_id"/>
+    <tableColumn id="2" xr3:uid="{9665E340-C35A-4AF6-A579-3C4549959807}" name="skills"/>
+    <tableColumn id="3" xr3:uid="{17381544-02D4-49EC-996D-7D74C03D8627}" name="skill_count"/>
+    <tableColumn id="4" xr3:uid="{5175B0B0-8321-43EF-B72E-7AB15F380A0E}" name="avg_salary"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2683,7 +5973,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{550D441F-795F-412B-9D47-A763F862A11C}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P34" sqref="P34"/>
     </sheetView>
   </sheetViews>
@@ -2890,4 +6180,307 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFEB1B06-C65B-43E2-80C4-685717837916}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="X53" sqref="X53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="3">
+        <v>92628</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="3">
+        <v>67031</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="3">
+        <v>57326</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="3">
+        <v>46554</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="3">
+        <v>39468</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75E7DCCE-E31D-419B-B7ED-2038682ACEF0}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S11" sqref="S11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2">
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3">
+        <v>179000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4">
+        <v>160515</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5">
+        <v>155486</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6">
+        <v>155000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7">
+        <v>149000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8">
+        <v>147633</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9">
+        <v>147500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10">
+        <v>146734</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11">
+        <v>138500</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{343D9BE0-78F8-44B4-B4CA-9528DA4C315A}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AC30" sqref="AC30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>98</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2">
+        <v>40</v>
+      </c>
+      <c r="D2">
+        <v>129999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>101</v>
+      </c>
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>125226</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>124686</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>99</v>
+      </c>
+      <c r="B5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5">
+        <v>24</v>
+      </c>
+      <c r="D5">
+        <v>120647</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>63</v>
+      </c>
+      <c r="B6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>118407</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>219</v>
+      </c>
+      <c r="B7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>117966</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>